<commit_message>
updated courts list full file again
</commit_message>
<xml_diff>
--- a/docassemble/VTSharedYMLFile/data/sources/courts_list_full.xlsx
+++ b/docassemble/VTSharedYMLFile/data/sources/courts_list_full.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtlegalaid-my.sharepoint.com/personal/ksurette_legalservicesvt_org/Documents/TIG 22/Docassemble guided interviews Suffolk project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{53F81566-F4D0-4366-90AE-5DA54A65EA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6BE0666-EF23-411A-96A8-E5E3F6EE2591}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{53F81566-F4D0-4366-90AE-5DA54A65EA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8282617-9972-42EE-BB09-EE5C943EE47D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F13D4BD2-1651-4B43-8F6C-36F85B10F0AA}"/>
   </bookViews>
@@ -886,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A491E8-E2DE-9A4E-A3B9-C224836C99FE}">
   <dimension ref="A1:T59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O47" sqref="O47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2698,7 +2698,7 @@
       <c r="G44" t="s">
         <v>127</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I44" s="5" t="s">
         <v>144</v>
       </c>
       <c r="J44" t="s">
@@ -2713,7 +2713,7 @@
       <c r="M44" t="s">
         <v>22</v>
       </c>
-      <c r="N44">
+      <c r="N44" s="7">
         <v>5401</v>
       </c>
       <c r="O44" t="s">
@@ -2739,7 +2739,7 @@
       <c r="G45" t="s">
         <v>130</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I45" s="5" t="s">
         <v>131</v>
       </c>
       <c r="J45" t="s">
@@ -2751,7 +2751,7 @@
       <c r="M45" t="s">
         <v>22</v>
       </c>
-      <c r="N45">
+      <c r="N45" s="7">
         <v>5001</v>
       </c>
       <c r="O45" t="s">
@@ -3344,8 +3344,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" display="AddisonUnit@vermont.gov" xr:uid="{CE067579-4D2A-4FB7-BC20-71CF63E84A64}"/>
-    <hyperlink ref="I3" r:id="rId2" display="BenningtonUnit@vermont.gov" xr:uid="{FB72F267-E788-4851-A3D1-CA77ACFF585C}"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{CE067579-4D2A-4FB7-BC20-71CF63E84A64}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{FB72F267-E788-4851-A3D1-CA77ACFF585C}"/>
     <hyperlink ref="I4" r:id="rId3" display="CaledoniaEssexUnit@vermont.gov" xr:uid="{1A175C18-6B0E-45DA-900D-8291E2C78C99}"/>
     <hyperlink ref="I5" r:id="rId4" display="ChittendenUnit@vermont.gov" xr:uid="{9FF34C42-4441-46C0-BE1D-9155E2E8825B}"/>
     <hyperlink ref="I6" r:id="rId5" display="CaledoniaEssexUnit@vermont.gov" xr:uid="{760AAC80-1B97-436E-AEB1-09E75778AC9D}"/>
@@ -3357,51 +3357,51 @@
     <hyperlink ref="I12" r:id="rId11" display="RutlandUnit@vermont.gov" xr:uid="{E84206E9-32FD-488A-9404-A74109553EE1}"/>
     <hyperlink ref="I13" r:id="rId12" display="WashingtonUnit@vermont.gov" xr:uid="{62688A28-3730-46D9-8F5B-6CB580AB3A11}"/>
     <hyperlink ref="I14" r:id="rId13" display="WindhamUnit@vermont.gov" xr:uid="{AE616A9A-A9CF-473C-AA71-EF580C860226}"/>
-    <hyperlink ref="I15" r:id="rId14" display="WindsorUnit@vermont.gov" xr:uid="{79E27C0A-1083-4C5E-B394-01C1BC9FC0CD}"/>
-    <hyperlink ref="I16" r:id="rId15" display="AddisonUnit@vermont.gov" xr:uid="{4A55FA55-EEB3-4B06-8E9A-C83765B14581}"/>
-    <hyperlink ref="I17" r:id="rId16" display="BenningtonUnit@vermont.gov" xr:uid="{F5846B64-7D2B-4EA9-A752-DEAE4E72E362}"/>
-    <hyperlink ref="I18" r:id="rId17" xr:uid="{A4A4A874-E4B7-44B8-9E90-89BB39E96775}"/>
-    <hyperlink ref="I19" r:id="rId18" xr:uid="{6A202E57-4DE0-4D16-9F4E-7D8F65CE1762}"/>
-    <hyperlink ref="I20" r:id="rId19" xr:uid="{0682AAD8-00E5-4949-B772-70778872FFF5}"/>
-    <hyperlink ref="I21" r:id="rId20" xr:uid="{8712C140-D413-43C0-A867-011098A3B272}"/>
-    <hyperlink ref="I22" r:id="rId21" xr:uid="{0D34FD78-2607-4346-AB53-AE0B6D796361}"/>
-    <hyperlink ref="I23" r:id="rId22" xr:uid="{92B4C53D-7BE3-46A3-B6C5-C07526084989}"/>
-    <hyperlink ref="I24" r:id="rId23" xr:uid="{A0D36FC9-2BD1-4ECB-A278-753DCCF813BC}"/>
-    <hyperlink ref="I25" r:id="rId24" xr:uid="{1BD2A3C4-BA91-459E-B929-C77E984B3450}"/>
-    <hyperlink ref="I26" r:id="rId25" xr:uid="{E6D72075-6EB0-4F34-A194-C1F9AB8E8F1A}"/>
-    <hyperlink ref="I27" r:id="rId26" xr:uid="{8D40A5D5-B35C-4505-B035-5AAB4A44A1BC}"/>
-    <hyperlink ref="I28" r:id="rId27" xr:uid="{09EFE2F4-2821-4608-B0B0-E0137AA308CD}"/>
-    <hyperlink ref="I29" r:id="rId28" xr:uid="{16F6DBC8-C336-483E-B9EF-76F76D347A6E}"/>
-    <hyperlink ref="I30" r:id="rId29" xr:uid="{0F7B39CE-DD14-43F4-A959-891D6B4E1F34}"/>
-    <hyperlink ref="I31" r:id="rId30" xr:uid="{6FC579A3-819C-47E6-9A7B-C93CAC63E5A3}"/>
-    <hyperlink ref="I32" r:id="rId31" xr:uid="{219729DB-1039-4400-9B07-43C2C104D9AD}"/>
-    <hyperlink ref="I33" r:id="rId32" xr:uid="{91FEC728-C373-46FD-B76E-96B37C0C0D09}"/>
-    <hyperlink ref="I34" r:id="rId33" xr:uid="{0BD2AB8E-3278-4694-9E73-822BAF35073A}"/>
-    <hyperlink ref="I35" r:id="rId34" xr:uid="{84CDACA3-ED0A-405E-9804-C8BAA8E75337}"/>
-    <hyperlink ref="I36" r:id="rId35" xr:uid="{1C2DB7AC-F3AE-41C9-AE84-2D800F417D82}"/>
-    <hyperlink ref="I37" r:id="rId36" xr:uid="{FBB062B1-C0B9-4A98-BBF1-F36C43FAE49B}"/>
-    <hyperlink ref="I38" r:id="rId37" xr:uid="{3DD10C8C-E6FD-41DF-853D-D761505E635F}"/>
-    <hyperlink ref="I39" r:id="rId38" xr:uid="{C0AF86C7-025C-4CE2-8B11-7CE370813380}"/>
-    <hyperlink ref="I40" r:id="rId39" xr:uid="{44AE4776-9A02-47E7-A3A9-773B01319A55}"/>
-    <hyperlink ref="I41" r:id="rId40" xr:uid="{85A98D47-0F16-4024-BDA1-203C9C7F5EAD}"/>
-    <hyperlink ref="I42" r:id="rId41" xr:uid="{7985C3BF-D1EC-4776-9D55-DFDCFB4FD907}"/>
-    <hyperlink ref="I43" r:id="rId42" xr:uid="{887F9765-37FE-436D-AD0B-EFBB5DC9E16B}"/>
-    <hyperlink ref="I45" r:id="rId43" xr:uid="{790534DE-D49A-4BA2-A92B-FD66D713D0F3}"/>
-    <hyperlink ref="I46" r:id="rId44" display="AddisonUnit@vermont.gov" xr:uid="{6F65162A-76DF-44FC-8F37-C22043850446}"/>
-    <hyperlink ref="I47" r:id="rId45" display="BenningtonUnit@vermont.gov" xr:uid="{77767542-E8F8-408E-9DE4-53EBC58FB08F}"/>
-    <hyperlink ref="I48" r:id="rId46" xr:uid="{A79A5CD5-9DD0-4BBC-916C-809348F5B64E}"/>
-    <hyperlink ref="I49" r:id="rId47" xr:uid="{A31BFBF8-D614-48C8-B837-4A739FFB1699}"/>
-    <hyperlink ref="I50" r:id="rId48" xr:uid="{F3F14201-F66D-4516-B4C4-26E10DC07E94}"/>
-    <hyperlink ref="I51" r:id="rId49" xr:uid="{EFE3A6D5-A378-4212-B347-070CD5782ABA}"/>
-    <hyperlink ref="I52" r:id="rId50" xr:uid="{A8A0E175-BD5D-4C83-95BC-F42E2BE75868}"/>
-    <hyperlink ref="I53" r:id="rId51" xr:uid="{75765CE9-BCD5-4D37-B03E-619896AAF600}"/>
-    <hyperlink ref="I54" r:id="rId52" xr:uid="{09157CB6-F34F-4AB2-8E4B-39713CD8E3F2}"/>
-    <hyperlink ref="I55" r:id="rId53" xr:uid="{921C2B89-E063-4064-AEF8-291B9236BB7F}"/>
-    <hyperlink ref="I56" r:id="rId54" xr:uid="{EFC0BB34-DA67-4F71-9200-F5F995EFB539}"/>
-    <hyperlink ref="I57" r:id="rId55" xr:uid="{98D10E1D-4A18-45EE-A025-C2EB7E3CAA3B}"/>
-    <hyperlink ref="I58" r:id="rId56" xr:uid="{04FC0544-87FB-4DA9-8C87-95BC2EFB7F62}"/>
-    <hyperlink ref="I59" r:id="rId57" xr:uid="{500D52E8-A4D4-4FDF-9C29-8FD1AB1FB9CC}"/>
-    <hyperlink ref="I44" r:id="rId58" display="https://www.vermontjudiciary.org/court-locations/EnvironmentalDivision@vtcourts.gov" xr:uid="{BE6A6C68-F953-4184-919E-05CAA10AF1B2}"/>
+    <hyperlink ref="I15" r:id="rId14" xr:uid="{79E27C0A-1083-4C5E-B394-01C1BC9FC0CD}"/>
+    <hyperlink ref="I17" r:id="rId15" display="BenningtonUnit@vermont.gov" xr:uid="{F5846B64-7D2B-4EA9-A752-DEAE4E72E362}"/>
+    <hyperlink ref="I18" r:id="rId16" xr:uid="{A4A4A874-E4B7-44B8-9E90-89BB39E96775}"/>
+    <hyperlink ref="I19" r:id="rId17" xr:uid="{6A202E57-4DE0-4D16-9F4E-7D8F65CE1762}"/>
+    <hyperlink ref="I20" r:id="rId18" xr:uid="{0682AAD8-00E5-4949-B772-70778872FFF5}"/>
+    <hyperlink ref="I21" r:id="rId19" xr:uid="{8712C140-D413-43C0-A867-011098A3B272}"/>
+    <hyperlink ref="I22" r:id="rId20" xr:uid="{0D34FD78-2607-4346-AB53-AE0B6D796361}"/>
+    <hyperlink ref="I23" r:id="rId21" xr:uid="{92B4C53D-7BE3-46A3-B6C5-C07526084989}"/>
+    <hyperlink ref="I24" r:id="rId22" xr:uid="{A0D36FC9-2BD1-4ECB-A278-753DCCF813BC}"/>
+    <hyperlink ref="I25" r:id="rId23" xr:uid="{1BD2A3C4-BA91-459E-B929-C77E984B3450}"/>
+    <hyperlink ref="I26" r:id="rId24" xr:uid="{E6D72075-6EB0-4F34-A194-C1F9AB8E8F1A}"/>
+    <hyperlink ref="I27" r:id="rId25" xr:uid="{8D40A5D5-B35C-4505-B035-5AAB4A44A1BC}"/>
+    <hyperlink ref="I28" r:id="rId26" xr:uid="{09EFE2F4-2821-4608-B0B0-E0137AA308CD}"/>
+    <hyperlink ref="I29" r:id="rId27" xr:uid="{16F6DBC8-C336-483E-B9EF-76F76D347A6E}"/>
+    <hyperlink ref="I31" r:id="rId28" xr:uid="{6FC579A3-819C-47E6-9A7B-C93CAC63E5A3}"/>
+    <hyperlink ref="I32" r:id="rId29" xr:uid="{219729DB-1039-4400-9B07-43C2C104D9AD}"/>
+    <hyperlink ref="I33" r:id="rId30" xr:uid="{91FEC728-C373-46FD-B76E-96B37C0C0D09}"/>
+    <hyperlink ref="I34" r:id="rId31" xr:uid="{0BD2AB8E-3278-4694-9E73-822BAF35073A}"/>
+    <hyperlink ref="I35" r:id="rId32" xr:uid="{84CDACA3-ED0A-405E-9804-C8BAA8E75337}"/>
+    <hyperlink ref="I36" r:id="rId33" xr:uid="{1C2DB7AC-F3AE-41C9-AE84-2D800F417D82}"/>
+    <hyperlink ref="I37" r:id="rId34" xr:uid="{FBB062B1-C0B9-4A98-BBF1-F36C43FAE49B}"/>
+    <hyperlink ref="I38" r:id="rId35" xr:uid="{3DD10C8C-E6FD-41DF-853D-D761505E635F}"/>
+    <hyperlink ref="I39" r:id="rId36" xr:uid="{C0AF86C7-025C-4CE2-8B11-7CE370813380}"/>
+    <hyperlink ref="I40" r:id="rId37" xr:uid="{44AE4776-9A02-47E7-A3A9-773B01319A55}"/>
+    <hyperlink ref="I41" r:id="rId38" xr:uid="{85A98D47-0F16-4024-BDA1-203C9C7F5EAD}"/>
+    <hyperlink ref="I42" r:id="rId39" xr:uid="{7985C3BF-D1EC-4776-9D55-DFDCFB4FD907}"/>
+    <hyperlink ref="I43" r:id="rId40" xr:uid="{887F9765-37FE-436D-AD0B-EFBB5DC9E16B}"/>
+    <hyperlink ref="I45" r:id="rId41" xr:uid="{790534DE-D49A-4BA2-A92B-FD66D713D0F3}"/>
+    <hyperlink ref="I47" r:id="rId42" display="BenningtonUnit@vermont.gov" xr:uid="{77767542-E8F8-408E-9DE4-53EBC58FB08F}"/>
+    <hyperlink ref="I48" r:id="rId43" xr:uid="{A79A5CD5-9DD0-4BBC-916C-809348F5B64E}"/>
+    <hyperlink ref="I49" r:id="rId44" xr:uid="{A31BFBF8-D614-48C8-B837-4A739FFB1699}"/>
+    <hyperlink ref="I50" r:id="rId45" xr:uid="{F3F14201-F66D-4516-B4C4-26E10DC07E94}"/>
+    <hyperlink ref="I51" r:id="rId46" xr:uid="{EFE3A6D5-A378-4212-B347-070CD5782ABA}"/>
+    <hyperlink ref="I52" r:id="rId47" xr:uid="{A8A0E175-BD5D-4C83-95BC-F42E2BE75868}"/>
+    <hyperlink ref="I53" r:id="rId48" xr:uid="{75765CE9-BCD5-4D37-B03E-619896AAF600}"/>
+    <hyperlink ref="I54" r:id="rId49" xr:uid="{09157CB6-F34F-4AB2-8E4B-39713CD8E3F2}"/>
+    <hyperlink ref="I55" r:id="rId50" xr:uid="{921C2B89-E063-4064-AEF8-291B9236BB7F}"/>
+    <hyperlink ref="I56" r:id="rId51" xr:uid="{EFC0BB34-DA67-4F71-9200-F5F995EFB539}"/>
+    <hyperlink ref="I57" r:id="rId52" xr:uid="{98D10E1D-4A18-45EE-A025-C2EB7E3CAA3B}"/>
+    <hyperlink ref="I58" r:id="rId53" xr:uid="{04FC0544-87FB-4DA9-8C87-95BC2EFB7F62}"/>
+    <hyperlink ref="I59" r:id="rId54" xr:uid="{500D52E8-A4D4-4FDF-9C29-8FD1AB1FB9CC}"/>
+    <hyperlink ref="I44" r:id="rId55" xr:uid="{BE6A6C68-F953-4184-919E-05CAA10AF1B2}"/>
+    <hyperlink ref="I16" r:id="rId56" xr:uid="{5830BA12-A226-46C8-9DC4-7E52B01732CB}"/>
+    <hyperlink ref="I30" r:id="rId57" xr:uid="{6C038597-579A-46D2-A6BB-0AE6B8405458}"/>
+    <hyperlink ref="I46" r:id="rId58" xr:uid="{85F665A1-D6D5-4734-8DF5-8CEAA44D01C4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId59"/>

</xml_diff>

<commit_message>
updated courts_list_full file to fix Newfane mailing address
</commit_message>
<xml_diff>
--- a/docassemble/VTSharedYMLFile/data/sources/courts_list_full.xlsx
+++ b/docassemble/VTSharedYMLFile/data/sources/courts_list_full.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtlegalaid-my.sharepoint.com/personal/ksurette_legalservicesvt_org/Documents/TIG 22/Docassemble guided interviews Suffolk project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksurette\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{53F81566-F4D0-4366-90AE-5DA54A65EA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49364260-E149-4326-BD9D-764F639C8F5D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604D16C7-3D2B-4DC2-8152-D396813C3EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F13D4BD2-1651-4B43-8F6C-36F85B10F0AA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F13D4BD2-1651-4B43-8F6C-36F85B10F0AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="151">
   <si>
     <t>name</t>
   </si>
@@ -904,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A491E8-E2DE-9A4E-A3B9-C224836C99FE}">
   <dimension ref="A1:T73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="H73" sqref="H73"/>
+    <sheetView tabSelected="1" topLeftCell="J30" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2064,9 +2064,6 @@
       <c r="S27" t="s">
         <v>101</v>
       </c>
-      <c r="T27" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -2104,6 +2101,9 @@
       </c>
       <c r="S28" t="s">
         <v>101</v>
+      </c>
+      <c r="T28" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
@@ -3276,9 +3276,6 @@
       </c>
       <c r="S57" t="s">
         <v>142</v>
-      </c>
-      <c r="T57" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>